<commit_message>
All loading tables by name
</commit_message>
<xml_diff>
--- a/test/templates/test-tables.xlsx
+++ b/test/templates/test-tables.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -491,7 +491,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>